<commit_message>
Update excel and txt file
</commit_message>
<xml_diff>
--- a/src/products/seznam-náhradního-spotřebního-materiálu.xlsx
+++ b/src/products/seznam-náhradního-spotřebního-materiálu.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="Produkty" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Čisticí prostředky, cyklokosmetika" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="test" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Kalkulačka nákladů" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Kalkulačka nákladů" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -107,11 +106,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -478,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -962,49 +961,6 @@
           <t>8595677700107</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>FD426G1652</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Desky brzdové GALFER FD426 E-bike/DH polymer, s pružinkou, pro SHIMANO M8120  </t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>541.0 Kč/Ks</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>541.0</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Ks</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2.0 Ks</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>ean</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1366,96 +1322,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="75" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="20" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>SKU</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Obrázek</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Název</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Cena za jednotku</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Skladem</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>EAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="20" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>FD426G1652</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Odkaz</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Desky brzdové GALFER FD426 E-bike/DH polymer, s pružinkou, pro SHIMANO M8120  </t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="inlineStr">
-        <is>
-          <t>541.0 Kč/Ks</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>2 Ks</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1536,387 +1402,388 @@
           <t>Cena celkem:</t>
         </is>
       </c>
-      <c r="I2" s="7">
+      <c r="I2">
         <f>SUM(F2:F21)</f>
         <v/>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
-      <c r="A3" s="8" t="inlineStr"/>
-      <c r="B3" s="8">
+      <c r="A3" s="7" t="inlineStr"/>
+      <c r="B3" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A3, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A3, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A3, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E3" s="8" t="inlineStr"/>
-      <c r="F3" s="9">
+      <c r="E3" s="7" t="inlineStr"/>
+      <c r="F3" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A3, "#"),Produkty!A:H, 5, FALSE)*E3, 0)</f>
         <v/>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="10" t="inlineStr"/>
-      <c r="B4" s="10">
+      <c r="A4" s="9" t="inlineStr"/>
+      <c r="B4" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A4, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A4, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A4, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E4" s="10" t="inlineStr"/>
-      <c r="F4" s="11">
+      <c r="E4" s="9" t="inlineStr"/>
+      <c r="F4" s="10">
         <f>IFERROR(VLOOKUP(TEXT(A4, "#"),Produkty!A:H, 5, FALSE)*E4, 0)</f>
         <v/>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
-      <c r="A5" s="8" t="inlineStr"/>
-      <c r="B5" s="8">
+      <c r="A5" s="7" t="inlineStr"/>
+      <c r="B5" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A5, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A5, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A5, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E5" s="8" t="inlineStr"/>
-      <c r="F5" s="9">
+      <c r="E5" s="7" t="inlineStr"/>
+      <c r="F5" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A5, "#"),Produkty!A:H, 5, FALSE)*E5, 0)</f>
         <v/>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
-      <c r="A6" s="10" t="inlineStr"/>
-      <c r="B6" s="10">
+      <c r="A6" s="9" t="inlineStr"/>
+      <c r="B6" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A6, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A6, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A6, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E6" s="10" t="inlineStr"/>
-      <c r="F6" s="11">
+      <c r="E6" s="9" t="inlineStr"/>
+      <c r="F6" s="10">
         <f>IFERROR(VLOOKUP(TEXT(A6, "#"),Produkty!A:H, 5, FALSE)*E6, 0)</f>
         <v/>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
-      <c r="A7" s="8" t="inlineStr"/>
-      <c r="B7" s="8">
+      <c r="A7" s="7" t="inlineStr"/>
+      <c r="B7" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A7, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A7, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A7, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E7" s="8" t="inlineStr"/>
-      <c r="F7" s="9">
+      <c r="E7" s="7" t="inlineStr"/>
+      <c r="F7" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A7, "#"),Produkty!A:H, 5, FALSE)*E7, 0)</f>
         <v/>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
-      <c r="A8" s="10" t="inlineStr"/>
-      <c r="B8" s="10">
+      <c r="A8" s="9" t="inlineStr"/>
+      <c r="B8" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A8, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A8, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A8, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E8" s="10" t="inlineStr"/>
-      <c r="F8" s="11">
+      <c r="E8" s="9" t="inlineStr"/>
+      <c r="F8" s="10">
         <f>IFERROR(VLOOKUP(TEXT(A8, "#"),Produkty!A:H, 5, FALSE)*E8, 0)</f>
         <v/>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
-      <c r="A9" s="8" t="inlineStr"/>
-      <c r="B9" s="8">
+      <c r="A9" s="7" t="inlineStr"/>
+      <c r="B9" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A9, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A9, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A9, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E9" s="8" t="inlineStr"/>
-      <c r="F9" s="9">
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A9, "#"),Produkty!A:H, 5, FALSE)*E9, 0)</f>
         <v/>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
-      <c r="A10" s="10" t="inlineStr"/>
-      <c r="B10" s="10">
+      <c r="A10" s="9" t="inlineStr"/>
+      <c r="B10" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A10, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A10, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A10, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E10" s="10" t="inlineStr"/>
-      <c r="F10" s="11">
+      <c r="E10" s="9" t="inlineStr"/>
+      <c r="F10" s="10">
         <f>IFERROR(VLOOKUP(TEXT(A10, "#"),Produkty!A:H, 5, FALSE)*E10, 0)</f>
         <v/>
       </c>
+      <c r="I10" s="11" t="n"/>
     </row>
     <row r="11" ht="20" customHeight="1">
-      <c r="A11" s="8" t="inlineStr"/>
-      <c r="B11" s="8">
+      <c r="A11" s="7" t="inlineStr"/>
+      <c r="B11" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A11, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A11, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A11, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E11" s="8" t="inlineStr"/>
-      <c r="F11" s="9">
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A11, "#"),Produkty!A:H, 5, FALSE)*E11, 0)</f>
         <v/>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
-      <c r="A12" s="10" t="inlineStr"/>
-      <c r="B12" s="10">
+      <c r="A12" s="9" t="inlineStr"/>
+      <c r="B12" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A12, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A12, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A12, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E12" s="10" t="inlineStr"/>
-      <c r="F12" s="11">
+      <c r="E12" s="9" t="inlineStr"/>
+      <c r="F12" s="10">
         <f>IFERROR(VLOOKUP(TEXT(A12, "#"),Produkty!A:H, 5, FALSE)*E12, 0)</f>
         <v/>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
-      <c r="A13" s="8" t="inlineStr"/>
-      <c r="B13" s="8">
+      <c r="A13" s="7" t="inlineStr"/>
+      <c r="B13" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A13, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A13, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A13, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E13" s="8" t="inlineStr"/>
-      <c r="F13" s="9">
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A13, "#"),Produkty!A:H, 5, FALSE)*E13, 0)</f>
         <v/>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
-      <c r="A14" s="10" t="inlineStr"/>
-      <c r="B14" s="10">
+      <c r="A14" s="9" t="inlineStr"/>
+      <c r="B14" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A14, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A14, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A14, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E14" s="10" t="inlineStr"/>
-      <c r="F14" s="11">
+      <c r="E14" s="9" t="inlineStr"/>
+      <c r="F14" s="10">
         <f>IFERROR(VLOOKUP(TEXT(A14, "#"),Produkty!A:H, 5, FALSE)*E14, 0)</f>
         <v/>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
-      <c r="A15" s="8" t="inlineStr"/>
-      <c r="B15" s="8">
+      <c r="A15" s="7" t="inlineStr"/>
+      <c r="B15" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A15, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A15, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A15, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E15" s="8" t="inlineStr"/>
-      <c r="F15" s="9">
+      <c r="E15" s="7" t="inlineStr"/>
+      <c r="F15" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A15, "#"),Produkty!A:H, 5, FALSE)*E15, 0)</f>
         <v/>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
-      <c r="A16" s="10" t="inlineStr"/>
-      <c r="B16" s="10">
+      <c r="A16" s="9" t="inlineStr"/>
+      <c r="B16" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A16, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A16, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A16, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E16" s="10" t="inlineStr"/>
-      <c r="F16" s="11">
+      <c r="E16" s="9" t="inlineStr"/>
+      <c r="F16" s="10">
         <f>IFERROR(VLOOKUP(TEXT(A16, "#"),Produkty!A:H, 5, FALSE)*E16, 0)</f>
         <v/>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
-      <c r="A17" s="8" t="inlineStr"/>
-      <c r="B17" s="8">
+      <c r="A17" s="7" t="inlineStr"/>
+      <c r="B17" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A17, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A17, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A17, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E17" s="8" t="inlineStr"/>
-      <c r="F17" s="9">
+      <c r="E17" s="7" t="inlineStr"/>
+      <c r="F17" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A17, "#"),Produkty!A:H, 5, FALSE)*E17, 0)</f>
         <v/>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
-      <c r="A18" s="10" t="inlineStr"/>
-      <c r="B18" s="10">
+      <c r="A18" s="9" t="inlineStr"/>
+      <c r="B18" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A18, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A18, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A18, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E18" s="10" t="inlineStr"/>
-      <c r="F18" s="11">
+      <c r="E18" s="9" t="inlineStr"/>
+      <c r="F18" s="10">
         <f>IFERROR(VLOOKUP(TEXT(A18, "#"),Produkty!A:H, 5, FALSE)*E18, 0)</f>
         <v/>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
-      <c r="A19" s="8" t="inlineStr"/>
-      <c r="B19" s="8">
+      <c r="A19" s="7" t="inlineStr"/>
+      <c r="B19" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A19, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A19, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A19, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E19" s="8" t="inlineStr"/>
-      <c r="F19" s="9">
+      <c r="E19" s="7" t="inlineStr"/>
+      <c r="F19" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A19, "#"),Produkty!A:H, 5, FALSE)*E19, 0)</f>
         <v/>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
-      <c r="A20" s="10" t="inlineStr"/>
-      <c r="B20" s="10">
+      <c r="A20" s="9" t="inlineStr"/>
+      <c r="B20" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A20, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A20, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <f>IFERROR(VLOOKUP(TEXT(A20, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E20" s="10" t="inlineStr"/>
-      <c r="F20" s="11">
+      <c r="E20" s="9" t="inlineStr"/>
+      <c r="F20" s="10">
         <f>IFERROR(VLOOKUP(TEXT(A20, "#"),Produkty!A:H, 5, FALSE)*E20, 0)</f>
         <v/>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
-      <c r="A21" s="8" t="inlineStr"/>
-      <c r="B21" s="8">
+      <c r="A21" s="7" t="inlineStr"/>
+      <c r="B21" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A21, "#"),Produkty!A:H, 2, FALSE), "")</f>
         <v/>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A21, "#"),Produkty!A:H, 7, FALSE), "")</f>
         <v/>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="7">
         <f>IFERROR(VLOOKUP(TEXT(A21, "#"),Produkty!A:H, 4, FALSE), "")</f>
         <v/>
       </c>
-      <c r="E21" s="8" t="inlineStr"/>
-      <c r="F21" s="9">
+      <c r="E21" s="7" t="inlineStr"/>
+      <c r="F21" s="8">
         <f>IFERROR(VLOOKUP(TEXT(A21, "#"),Produkty!A:H, 5, FALSE)*E21, 0)</f>
         <v/>
       </c>

</xml_diff>